<commit_message>
DMB-Infos angepasst, engl. Ü. fehlt noch
</commit_message>
<xml_diff>
--- a/data/study/study.xlsx
+++ b/data/study/study.xlsx
@@ -15,12 +15,12 @@
     <definedName name="_ftn1" localSheetId="0">study!$K$5</definedName>
     <definedName name="_ftnref1" localSheetId="0">study!$K$2</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
   <si>
     <t>title.de</t>
   </si>
@@ -160,9 +160,6 @@
     <t>Educational paths of school leavers with a higher education entrance qualification - Panel Study of School Leavers with a Higher Education Entrance Qualification 2008</t>
   </si>
   <si>
-    <t>Heine, C., Quast, H., Spangenberg, H., Lörz, M., Scheller, P. &amp; Willich, J. (2014): Educational paths of school leavers with a higher education entrance qualification - DZHW Panel Study of School Leavers with a Higher Education Entrance Qualification 2008. Edited by Daniel, A., Hoffstätter, U., Huß, B. &amp; Scheller, P., doi: 10.21249/DZHW:gsl2008:1.0.0, dataset, released 2017. Hannover: FDZ-DZHW.</t>
-  </si>
-  <si>
     <t>filename</t>
   </si>
   <si>
@@ -190,9 +187,6 @@
     <t>Method Report</t>
   </si>
   <si>
-    <t>Daten- und Methodenbericht zum Studienberechtigtenpanel 2008</t>
-  </si>
-  <si>
     <t>Mareike</t>
   </si>
   <si>
@@ -200,13 +194,16 @@
   </si>
   <si>
     <t>Daten- und Methodenbericht</t>
+  </si>
+  <si>
+    <t>Daten- und Methodenbericht zu den Erhebungen des Studienberechtigtenjahrgangs 2008 (1. bis 3. Befragungswelle). Version 1.0.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -234,12 +231,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -275,7 +266,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -288,7 +279,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -595,7 +585,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,7 +671,7 @@
       <c r="C2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -705,9 +695,7 @@
       <c r="K2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="L2" s="3"/>
       <c r="M2" s="1" t="s">
         <v>40</v>
       </c>
@@ -780,7 +768,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
         <v>33</v>
@@ -824,7 +812,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,16 +828,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>49</v>
-      </c>
-      <c r="D1" t="s">
-        <v>50</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -858,30 +846,30 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" t="s">
         <v>53</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Übersetzung und kleine Korrekturen
</commit_message>
<xml_diff>
--- a/data/study/study.xlsx
+++ b/data/study/study.xlsx
@@ -15,7 +15,7 @@
     <definedName name="_ftn1" localSheetId="0">study!$K$5</definedName>
     <definedName name="_ftnref1" localSheetId="0">study!$K$2</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -58,12 +58,6 @@
     <t>citationHint.en</t>
   </si>
   <si>
-    <t>Deutsches Zentrum für Hochschul- und Wissenschaftsforschung</t>
-  </si>
-  <si>
-    <t>Bundesministerium für Bildung und Forschung</t>
-  </si>
-  <si>
     <t>DZHW-Studienberechtigtenbefragungen</t>
   </si>
   <si>
@@ -190,26 +184,39 @@
     <t>Mareike</t>
   </si>
   <si>
-    <t xml:space="preserve">Data and Methods Report on the Panel Study of School Leavers </t>
-  </si>
-  <si>
     <t>Daten- und Methodenbericht</t>
   </si>
   <si>
     <t>Daten- und Methodenbericht zu den Erhebungen des Studienberechtigtenjahrgangs 2008 (1. bis 3. Befragungswelle). Version 1.0.0</t>
+  </si>
+  <si>
+    <t>Bundesministerium für Bildung und Forschung (BMBF)</t>
+  </si>
+  <si>
+    <t>Deutsches Zentrum für Hochschul- und Wissenschaftsforschung (DZHW)</t>
+  </si>
+  <si>
+    <t>Data and methods report for the surveys on School Leavers with a Higher Education Entrance Qualification of the year 2008</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -232,8 +239,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,14 +259,8 @@
         <bgColor rgb="FFFFCCCC"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -261,25 +268,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Erklärender Text 2" xfId="1"/>
@@ -582,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,65 +679,68 @@
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="286.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="H2" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -733,69 +766,69 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -809,10 +842,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,56 +854,59 @@
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="52.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
         <v>46</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>47</v>
       </c>
-      <c r="C1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" t="s">
-        <v>53</v>
-      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
gsl2008, ssy19, phd2014 MethodReport_en
</commit_message>
<xml_diff>
--- a/data/study/study.xlsx
+++ b/data/study/study.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
   <si>
     <t>title.de</t>
   </si>
@@ -209,6 +209,12 @@
   </si>
   <si>
     <t>studySeries.en</t>
+  </si>
+  <si>
+    <t>gsl2008_MethodReport_en.pdf</t>
+  </si>
+  <si>
+    <t>DZHW Panel Study of School Leavers with a Higher Education Entrance Qualification 2008</t>
   </si>
 </sst>
 </file>
@@ -622,7 +628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -842,10 +848,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,31 +911,54 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>54</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>56</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>55</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>59</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E6" s="4"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>